<commit_message>
finance gsdp - current
</commit_message>
<xml_diff>
--- a/app/datasets/finance/finance_overall.xlsx
+++ b/app/datasets/finance/finance_overall.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\econ_gju\datasets\finance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Music\econ-dashboard\app\datasets\finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB644F0-9EBC-4C03-B15D-BC9656BCB7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B28D83-D769-4A0D-AFA6-A1D4A73DF836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-114" yWindow="-114" windowWidth="19704" windowHeight="10736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,17 +112,17 @@
     <t>Total Revenue Expenditure</t>
   </si>
   <si>
-    <t>SGDP</t>
-  </si>
-  <si>
     <t>Total Tax to GSDP Ratio</t>
+  </si>
+  <si>
+    <t>GDP (Current Prices)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +149,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,10 +176,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -187,9 +197,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8210356F-98F5-4D6F-8AC3-46DF02CD028A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -485,11 +506,11 @@
     <col min="8" max="8" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,13 +542,13 @@
         <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -558,15 +579,15 @@
       <c r="J2" s="1">
         <v>17526.87</v>
       </c>
-      <c r="K2">
-        <v>212193.67</v>
+      <c r="K2" s="8">
+        <v>151595.9</v>
       </c>
       <c r="L2">
         <f>D2/K2 * 100</f>
-        <v>6.245322963686899</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.7417799557903617</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -597,15 +618,15 @@
       <c r="J3" s="1">
         <v>20534.73</v>
       </c>
-      <c r="K3">
-        <v>229528.26</v>
+      <c r="K3" s="9">
+        <v>182522.15</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L15" si="0">D3/K3 * 100</f>
-        <v>5.8293039820020418</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.3305623454468405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -636,15 +657,18 @@
       <c r="J4" s="1">
         <v>25257.38</v>
       </c>
-      <c r="K4">
-        <v>256431.19</v>
+      <c r="K4" s="8">
+        <v>223600.25</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>5.8471709311180122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.7057035938018847</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -675,15 +699,18 @@
       <c r="J5" s="1">
         <v>28310.19</v>
       </c>
-      <c r="K5">
-        <v>275428.32</v>
+      <c r="K5" s="8">
+        <v>260621.28</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>6.9317926348314503</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.3256182304069721</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -714,15 +741,18 @@
       <c r="J6" s="1">
         <v>32014.89</v>
       </c>
-      <c r="K6">
-        <v>297538.52</v>
+      <c r="K6" s="8">
+        <v>297538.52068239864</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>7.7573182793273272</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.7573182615360743</v>
+      </c>
+      <c r="N6" s="7"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -753,15 +783,18 @@
       <c r="J7" s="1">
         <v>38071.72</v>
       </c>
-      <c r="K7">
-        <v>320911.90999999997</v>
+      <c r="K7" s="8">
+        <v>347032.01266926259</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>8.2954633874448618</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.6710876887807924</v>
+      </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -792,15 +825,18 @@
       <c r="J8" s="1">
         <v>41887.1</v>
       </c>
-      <c r="K8">
-        <v>347506.61</v>
+      <c r="K8" s="8">
+        <v>399268.11618977698</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>8.319220172531395</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.2407083931186733</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -831,15 +867,18 @@
       <c r="J9" s="4">
         <v>49117.87</v>
       </c>
-      <c r="K9">
-        <v>370534.51</v>
+      <c r="K9" s="8">
+        <v>437144.71134774183</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>8.4155886046889385</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.1332579785449308</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -870,15 +909,18 @@
       <c r="J10" s="4">
         <v>59235.7</v>
       </c>
-      <c r="K10">
-        <v>413404.79</v>
+      <c r="K10" s="8">
+        <v>495504.10640162957</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>8.8110517538996103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.3511620851181316</v>
+      </c>
+      <c r="N10" s="7"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -909,15 +951,18 @@
       <c r="J11" s="4">
         <v>68403.429999999993</v>
       </c>
-      <c r="K11">
-        <v>456709.11</v>
+      <c r="K11" s="8">
+        <v>561424.1711553171</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>8.8947557888652593</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.2357340647454365</v>
+      </c>
+      <c r="N11" s="7"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -948,15 +993,18 @@
       <c r="J12" s="4">
         <v>73257.350000000006</v>
       </c>
-      <c r="K12">
-        <v>487273.84</v>
+      <c r="K12" s="8">
+        <v>644963.22063958389</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>9.9321769459242866</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.5038232338282409</v>
+      </c>
+      <c r="N12" s="7"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -987,15 +1035,18 @@
       <c r="J13" s="4">
         <v>77155.539999999994</v>
       </c>
-      <c r="K13">
-        <v>517079.99</v>
+      <c r="K13" s="8">
+        <v>704957.37832466571</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>9.8313493043890556</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.2112075939699842</v>
+      </c>
+      <c r="N13" s="7"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1026,15 +1077,18 @@
       <c r="J14" s="4">
         <v>92256.1</v>
       </c>
-      <c r="K14">
-        <v>559705</v>
+      <c r="K14" s="8">
+        <v>780612.35380656121</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>9.8183096452595571</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.0398027563906203</v>
+      </c>
+      <c r="N14" s="7"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1065,13 +1119,77 @@
       <c r="J15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K15">
-        <v>528069.75</v>
+      <c r="K15" s="8">
+        <v>764872.40858543455</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>11.472058378651685</v>
-      </c>
+        <v>7.9203366888391677</v>
+      </c>
+      <c r="N15" s="7"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="7"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I19" s="7"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
gdp and finance changes
</commit_message>
<xml_diff>
--- a/app/datasets/finance/finance_overall.xlsx
+++ b/app/datasets/finance/finance_overall.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Music\econ-dashboard\app\datasets\finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D5A7D0-AAB9-48A0-B7F2-767DE931DF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4205799-D795-4101-B04B-64E640DA04DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="19704" windowHeight="10736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-114" yWindow="-114" windowWidth="19704" windowHeight="10736" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>Year</t>
   </si>
@@ -172,14 +173,35 @@
     <t>State's Own Total Non-Tax Revenue (₹ Crores)</t>
   </si>
   <si>
-    <t>State's Own Non-Tax Revenue to GDP Ratio</t>
+    <t>State's Own -Tax Revenue to GDP Ratio</t>
+  </si>
+  <si>
+    <t>1980-81</t>
+  </si>
+  <si>
+    <t>1981-82</t>
+  </si>
+  <si>
+    <t>1982-83</t>
+  </si>
+  <si>
+    <t>1983-84</t>
+  </si>
+  <si>
+    <t>1984-85</t>
+  </si>
+  <si>
+    <t>Lakhs</t>
+  </si>
+  <si>
+    <t>Crores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,8 +358,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,6 +551,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -679,7 +721,7 @@
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -696,6 +738,47 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1021,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1118,7 @@
     <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40" bestFit="1" customWidth="1"/>
   </cols>
@@ -1065,7 +1148,7 @@
       <c r="H1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="7" t="s">
         <v>44</v>
       </c>
       <c r="J1" s="4" t="s">
@@ -1100,16 +1183,16 @@
       <c r="H2" s="3">
         <v>258.12</v>
       </c>
-      <c r="I2" s="3">
-        <v>7570.88</v>
+      <c r="I2" s="20">
+        <v>6551.93</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ref="J2:J23" si="0">D2/I2 * 100</f>
-        <v>7.7561657297434392</v>
+        <v>8.9623973394099146</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2:K23" si="1">E2/I2 * 100</f>
-        <v>4.928357073418149</v>
+        <v>5.6948105367426081</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1137,16 +1220,16 @@
       <c r="H3" s="3">
         <v>296.62</v>
       </c>
-      <c r="I3" s="3">
-        <v>7960.06</v>
+      <c r="I3" s="20">
+        <v>6888.73</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="0"/>
-        <v>8.3299623369673093</v>
+        <v>9.6254316833436651</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="1"/>
-        <v>5.8681718479508946</v>
+        <v>6.7807854277929316</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1174,16 +1257,16 @@
       <c r="H4" s="3">
         <v>378</v>
       </c>
-      <c r="I4" s="3">
-        <v>8942.4500000000007</v>
+      <c r="I4" s="20">
+        <v>7738.9</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="0"/>
-        <v>8.6320862850784739</v>
+        <v>9.9745441858662094</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="1"/>
-        <v>5.9482580277217085</v>
+        <v>6.8733282507849953</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1214,16 +1297,16 @@
       <c r="H5" s="3">
         <v>354.71</v>
       </c>
-      <c r="I5" s="3">
-        <v>11572.48</v>
+      <c r="I5" s="20">
+        <v>10014.959999999999</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="0"/>
-        <v>7.9155893982966488</v>
+        <v>9.146616661474436</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="1"/>
-        <v>4.5370568797699367</v>
+        <v>5.2426569851502149</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1254,16 +1337,16 @@
       <c r="H6" s="3">
         <v>445.93</v>
       </c>
-      <c r="I6" s="3">
-        <v>12880.14</v>
+      <c r="I6" s="20">
+        <v>11146.63</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="0"/>
-        <v>8.2625654690088766</v>
+        <v>9.5475493489960641</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="1"/>
-        <v>4.2158703243908846</v>
+        <v>4.8715172208999489</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="1"/>
@@ -1294,16 +1377,16 @@
       <c r="H7" s="3">
         <v>511.1</v>
       </c>
-      <c r="I7" s="3">
-        <v>15757.15</v>
+      <c r="I7" s="20">
+        <v>13636.43</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="0"/>
-        <v>7.9674306584629848</v>
+        <v>9.2065151949593851</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="1"/>
-        <v>4.1757551333838929</v>
+        <v>4.8251631842058371</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="1"/>
@@ -1334,16 +1417,16 @@
       <c r="H8" s="3">
         <v>546.1</v>
       </c>
-      <c r="I8" s="3">
-        <v>18880.310000000001</v>
+      <c r="I8" s="20">
+        <v>16339.25</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="0"/>
-        <v>8.0488614858548395</v>
+        <v>9.3006104931376896</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="1"/>
-        <v>3.8248312660120511</v>
+        <v>4.4196643052771698</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="1"/>
@@ -1374,16 +1457,16 @@
       <c r="H9" s="3">
         <v>460.27</v>
       </c>
-      <c r="I9" s="3">
-        <v>20040.509999999998</v>
+      <c r="I9" s="20">
+        <v>17343.3</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="0"/>
-        <v>8.5267790091170337</v>
+        <v>9.8528538398113383</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="1"/>
-        <v>3.3373901163193955</v>
+        <v>3.8564171755086982</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="1"/>
@@ -1414,16 +1497,16 @@
       <c r="H10" s="3">
         <v>1340.55</v>
       </c>
-      <c r="I10" s="3">
-        <v>23710.04</v>
+      <c r="I10" s="20">
+        <v>22131.3</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="0"/>
-        <v>7.8926901852548541</v>
+        <v>8.4557165643229268</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="1"/>
-        <v>6.7907519346234748</v>
+        <v>7.2751713636343096</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="1"/>
@@ -1454,16 +1537,16 @@
       <c r="H11" s="3">
         <v>3473.41</v>
       </c>
-      <c r="I11" s="3">
-        <v>28116.94</v>
+      <c r="I11" s="20">
+        <v>26244.77</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="0"/>
-        <v>7.8422474138366409</v>
+        <v>8.401673933511324</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="1"/>
-        <v>13.078983701640365</v>
+        <v>14.011972671126474</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="1"/>
@@ -1494,16 +1577,16 @@
       <c r="H12" s="3">
         <v>2186.81</v>
       </c>
-      <c r="I12" s="3">
-        <v>31913.919999999998</v>
+      <c r="I12" s="20">
+        <v>29788.93</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="0"/>
-        <v>7.9257891227401709</v>
+        <v>8.4911744060629228</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="1"/>
-        <v>7.787510904332656</v>
+        <v>8.3430321263637204</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="1"/>
@@ -1534,16 +1617,16 @@
       <c r="H13" s="3">
         <v>3132.67</v>
       </c>
-      <c r="I13" s="3">
-        <v>38184.93</v>
+      <c r="I13" s="20">
+        <v>35642.379999999997</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="0"/>
-        <v>6.7435242123005059</v>
+        <v>7.2245736676394774</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="1"/>
-        <v>9.096049148184898</v>
+        <v>9.7449160241263346</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="1"/>
@@ -1574,16 +1657,16 @@
       <c r="H14" s="3">
         <v>2631.1</v>
       </c>
-      <c r="I14" s="3">
-        <v>41406.1</v>
+      <c r="I14" s="20">
+        <v>38649.07</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="0"/>
-        <v>7.0229748756825696</v>
+        <v>7.5239585325080265</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="1"/>
-        <v>7.2207476676141926</v>
+        <v>7.7358394393448533</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="1"/>
@@ -1614,16 +1697,16 @@
       <c r="H15" s="3">
         <v>1518.02</v>
       </c>
-      <c r="I15" s="3">
-        <v>46759.48</v>
+      <c r="I15" s="20">
+        <v>43645.99</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="0"/>
-        <v>7.6982464304564537</v>
+        <v>8.2474014222154199</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="1"/>
-        <v>4.0185006334544351</v>
+        <v>4.3051606802824267</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="1"/>
@@ -1654,16 +1737,16 @@
       <c r="H16" s="3">
         <v>1259.06</v>
       </c>
-      <c r="I16" s="3">
-        <v>52398.92</v>
+      <c r="I16" s="20">
+        <v>48909.93</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="0"/>
-        <v>7.7155788707095496</v>
+        <v>8.2659697120809614</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="1"/>
-        <v>3.2899151356554674</v>
+        <v>3.5246012415065815</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1694,16 +1777,16 @@
       <c r="H17" s="3">
         <v>1439.3899999999999</v>
       </c>
-      <c r="I17" s="3">
-        <v>59343.08</v>
+      <c r="I17" s="20">
+        <v>55005.45</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="0"/>
-        <v>7.8465088094517492</v>
+        <v>8.4652702595833684</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>3.2312613366208831</v>
+        <v>3.4860727437008512</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1738,16 +1821,16 @@
       <c r="H18" s="3">
         <v>1666.0700000000002</v>
       </c>
-      <c r="I18" s="3">
-        <v>66810.899999999994</v>
+      <c r="I18" s="20">
+        <v>60561.440000000002</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="0"/>
-        <v>8.1146040541288933</v>
+        <v>8.9519667960339131</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>3.2616085099886396</v>
+        <v>3.5981806245029837</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1782,16 +1865,16 @@
       <c r="H19" s="3">
         <v>1807.85</v>
       </c>
-      <c r="I19" s="3">
-        <v>73973.56</v>
+      <c r="I19" s="20">
+        <v>66175.429999999993</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="0"/>
-        <v>8.5250324575429381</v>
+        <v>9.5296245147179253</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>3.1778246173362481</v>
+        <v>3.5523003023932</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1826,16 +1909,16 @@
       <c r="H20" s="3">
         <v>2223.06</v>
       </c>
-      <c r="I20" s="3">
-        <v>84513.38</v>
+      <c r="I20" s="20">
+        <v>73960.740000000005</v>
       </c>
       <c r="J20" s="5">
         <f t="shared" si="0"/>
-        <v>8.2221300343211929</v>
+        <v>9.3952548338483357</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>3.4251144611657938</v>
+        <v>3.9138061625667881</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1870,16 +1953,16 @@
       <c r="H21" s="3">
         <v>2544.37</v>
       </c>
-      <c r="I21" s="3">
-        <v>95426.35</v>
+      <c r="I21" s="10">
+        <v>95795.12</v>
       </c>
       <c r="J21" s="5">
         <f t="shared" si="0"/>
-        <v>8.445811874812355</v>
+        <v>8.4132991325654167</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>3.2376068035715493</v>
+        <v>3.2251434102279952</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1907,16 +1990,16 @@
       <c r="H22" s="3">
         <v>2458.5700000000002</v>
       </c>
-      <c r="I22" s="3">
-        <v>108465.42</v>
+      <c r="I22" s="10">
+        <v>108884.57</v>
       </c>
       <c r="J22" s="5">
         <f t="shared" si="0"/>
-        <v>9.4773246625514371</v>
+        <v>9.440841801551862</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>3.2947827980567448</v>
+        <v>3.2820995665409707</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1944,16 +2027,16 @@
       <c r="H23" s="3">
         <v>4590.7699999999995</v>
       </c>
-      <c r="I23" s="3">
-        <v>128236.78</v>
+      <c r="I23" s="10">
+        <v>128732.34</v>
       </c>
       <c r="J23" s="5">
         <f t="shared" si="0"/>
-        <v>9.5318987267147541</v>
+        <v>9.495205322920409</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>4.4675404357470621</v>
+        <v>4.4503424702759231</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1981,16 +2064,16 @@
       <c r="H24" s="3">
         <v>5097.08</v>
       </c>
-      <c r="I24" s="3">
-        <v>151012.32999999999</v>
+      <c r="I24" s="10">
+        <v>151595.9</v>
       </c>
       <c r="J24" s="5">
-        <f>D24/I24 * 100</f>
-        <v>8.7755615716941797</v>
+        <f t="shared" ref="J24:J37" si="2">D24/I24 * 100</f>
+        <v>8.7417799557903617</v>
       </c>
       <c r="K24" s="5">
-        <f>E24/I24 * 100</f>
-        <v>3.3752740587473884</v>
+        <f t="shared" ref="K24:K37" si="3">E24/I24 * 100</f>
+        <v>3.3622809060139489</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2018,16 +2101,16 @@
       <c r="H25" s="3">
         <v>3238.45</v>
       </c>
-      <c r="I25" s="3">
-        <v>181819.53</v>
+      <c r="I25" s="10">
+        <v>182522.15</v>
       </c>
       <c r="J25" s="5">
-        <f>D25/I25 * 100</f>
-        <v>7.3588904338274332</v>
+        <f t="shared" si="2"/>
+        <v>7.3305623454468405</v>
       </c>
       <c r="K25" s="5">
-        <f>E25/I25 * 100</f>
-        <v>1.7811342928892182</v>
+        <f t="shared" si="3"/>
+        <v>1.7742778068305682</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2055,16 +2138,16 @@
       <c r="H26" s="3">
         <v>2741.4</v>
       </c>
-      <c r="I26" s="3">
-        <v>222739.49</v>
+      <c r="I26" s="10">
+        <v>223600.25</v>
       </c>
       <c r="J26" s="5">
-        <f>D26/I26 * 100</f>
-        <v>6.7316172807974013</v>
+        <f t="shared" si="2"/>
+        <v>6.7057035938018847</v>
       </c>
       <c r="K26" s="5">
-        <f>E26/I26 * 100</f>
-        <v>1.2307651418255472</v>
+        <f t="shared" si="3"/>
+        <v>1.2260272517584394</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2092,16 +2175,16 @@
       <c r="H27" s="3">
         <v>3420.94</v>
       </c>
-      <c r="I27" s="3">
-        <v>259618.01</v>
+      <c r="I27" s="10">
+        <v>260621.28</v>
       </c>
       <c r="J27" s="5">
-        <f>D27/I27 * 100</f>
-        <v>7.3539274105059187</v>
+        <f t="shared" si="2"/>
+        <v>7.3256182304069721</v>
       </c>
       <c r="K27" s="5">
-        <f>E27/I27 * 100</f>
-        <v>1.3176820822253432</v>
+        <f t="shared" si="3"/>
+        <v>1.3126096226678037</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2129,16 +2212,16 @@
       <c r="H28" s="3">
         <v>4721.6499999999996</v>
       </c>
-      <c r="I28" s="3">
-        <v>297538.52</v>
+      <c r="I28" s="21">
+        <v>297538.52068239864</v>
       </c>
       <c r="J28" s="5">
-        <f>D28/I28 * 100</f>
-        <v>7.7573182793273272</v>
+        <f t="shared" si="2"/>
+        <v>7.7573182615360743</v>
       </c>
       <c r="K28" s="5">
-        <f>E28/I28 * 100</f>
-        <v>1.5869037729971902</v>
+        <f t="shared" si="3"/>
+        <v>1.5869037693576584</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2166,16 +2249,16 @@
       <c r="H29" s="3">
         <v>4673.1499999999996</v>
       </c>
-      <c r="I29" s="3">
-        <v>347032.01</v>
+      <c r="I29" s="21">
+        <v>347032.01266926259</v>
       </c>
       <c r="J29" s="5">
-        <f>D29/I29 * 100</f>
-        <v>7.6710877477844193</v>
+        <f t="shared" si="2"/>
+        <v>7.6710876887807924</v>
       </c>
       <c r="K29" s="5">
-        <f>E29/I29 * 100</f>
-        <v>1.3466048852381081</v>
+        <f t="shared" si="3"/>
+        <v>1.3466048748804411</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2203,16 +2286,16 @@
       <c r="H30" s="3">
         <v>4975.0600000000004</v>
       </c>
-      <c r="I30" s="3">
-        <v>399268.12</v>
+      <c r="I30" s="21">
+        <v>399268.11618977698</v>
       </c>
       <c r="J30" s="5">
-        <f>D30/I30 * 100</f>
-        <v>7.2407083240204599</v>
+        <f t="shared" si="2"/>
+        <v>7.2407083931186733</v>
       </c>
       <c r="K30" s="5">
-        <f>E30/I30 * 100</f>
-        <v>1.2460448883321815</v>
+        <f t="shared" si="3"/>
+        <v>1.2460449002232108</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2240,16 +2323,16 @@
       <c r="H31" s="3">
         <v>4613.12</v>
       </c>
-      <c r="I31" s="3">
-        <v>437144.71</v>
+      <c r="I31" s="21">
+        <v>437144.71134774183</v>
       </c>
       <c r="J31" s="5">
-        <f>D31/I31 * 100</f>
-        <v>7.1332580005371664</v>
+        <f t="shared" si="2"/>
+        <v>7.1332579785449308</v>
       </c>
       <c r="K31" s="5">
-        <f>E31/I31 * 100</f>
-        <v>1.0552844160003674</v>
+        <f t="shared" si="3"/>
+        <v>1.0552844127468659</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2277,16 +2360,16 @@
       <c r="H32" s="3">
         <v>4752.49</v>
       </c>
-      <c r="I32" s="3">
-        <v>495504.11</v>
+      <c r="I32" s="21">
+        <v>495504.10640162957</v>
       </c>
       <c r="J32" s="5">
-        <f>D32/I32 * 100</f>
-        <v>7.3511620317337014</v>
+        <f t="shared" si="2"/>
+        <v>7.3511620851181316</v>
       </c>
       <c r="K32" s="5">
-        <f>E32/I32 * 100</f>
-        <v>0.95912221595901592</v>
+        <f t="shared" si="3"/>
+        <v>0.95912222292419935</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2314,16 +2397,16 @@
       <c r="H33" s="3">
         <v>6196.09</v>
       </c>
-      <c r="I33" s="3">
-        <v>561424.17000000004</v>
+      <c r="I33" s="21">
+        <v>561424.1711553171</v>
       </c>
       <c r="J33" s="5">
-        <f>D33/I33 * 100</f>
-        <v>7.2357340796353666</v>
+        <f t="shared" si="2"/>
+        <v>7.2357340647454365</v>
       </c>
       <c r="K33" s="5">
-        <f>E33/I33 * 100</f>
-        <v>1.1036379142707731</v>
+        <f t="shared" si="3"/>
+        <v>1.1036379119996709</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2351,16 +2434,16 @@
       <c r="H34" s="3">
         <v>9112.85</v>
       </c>
-      <c r="I34" s="3">
-        <v>644963.22</v>
+      <c r="I34" s="21">
+        <v>644963.22063958389</v>
       </c>
       <c r="J34" s="5">
-        <f>D34/I34 * 100</f>
-        <v>7.5038232412694787</v>
+        <f t="shared" si="2"/>
+        <v>7.5038232338282409</v>
       </c>
       <c r="K34" s="5">
-        <f>E34/I34 * 100</f>
-        <v>1.4129255308543021</v>
+        <f t="shared" si="3"/>
+        <v>1.4129255294531611</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2388,16 +2471,16 @@
       <c r="H35" s="3">
         <v>7975.64</v>
       </c>
-      <c r="I35" s="3">
-        <v>704957.38</v>
+      <c r="I35" s="21">
+        <v>704957.37832466571</v>
       </c>
       <c r="J35" s="5">
-        <f>D35/I35 * 100</f>
-        <v>7.2112075768325177</v>
+        <f t="shared" si="2"/>
+        <v>7.2112075939699842</v>
       </c>
       <c r="K35" s="5">
-        <f>E35/I35 * 100</f>
-        <v>1.1313648493189759</v>
+        <f t="shared" si="3"/>
+        <v>1.1313648520076693</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2425,16 +2508,16 @@
       <c r="H36" s="3">
         <v>10135.09</v>
       </c>
-      <c r="I36" s="3">
-        <v>780612.35</v>
+      <c r="I36" s="21">
+        <v>780612.35380656121</v>
       </c>
       <c r="J36" s="5">
-        <f>D36/I36 * 100</f>
-        <v>7.0398027907193628</v>
+        <f t="shared" si="2"/>
+        <v>7.0398027563906203</v>
       </c>
       <c r="K36" s="5">
-        <f>E36/I36 * 100</f>
-        <v>1.2983512238821229</v>
+        <f t="shared" si="3"/>
+        <v>1.2983512175508709</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2462,16 +2545,16 @@
       <c r="H37" s="3">
         <v>15428.22</v>
       </c>
-      <c r="I37" s="3">
-        <v>764872.41</v>
+      <c r="I37" s="21">
+        <v>764872.40858543455</v>
       </c>
       <c r="J37" s="5">
-        <f>D37/I37 * 100</f>
-        <v>7.9203366741911889</v>
+        <f t="shared" si="2"/>
+        <v>7.9203366888391677</v>
       </c>
       <c r="K37" s="5">
-        <f>E37/I37 * 100</f>
-        <v>2.0170972044866931</v>
+        <f t="shared" si="3"/>
+        <v>2.0170972082171406</v>
       </c>
     </row>
   </sheetData>
@@ -2479,4 +2562,732 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5F57DC9-AD3D-491D-ACDA-1FB075C892F0}">
+  <dimension ref="A1:S42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C2:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="10.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="13"/>
+    <col min="8" max="8" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9">
+        <v>338641</v>
+      </c>
+      <c r="C2" s="9">
+        <f>B2/100</f>
+        <v>3386.41</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="9">
+        <v>391078</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C14" si="0">B3/100</f>
+        <v>3910.78</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="9">
+        <v>448492</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="0"/>
+        <v>4484.92</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="9">
+        <v>488972</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="0"/>
+        <v>4889.72</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="9">
+        <v>538192</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>5381.92</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="9">
+        <v>655193</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>6551.93</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="9">
+        <v>688873</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>6888.73</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="9">
+        <v>773890</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>7738.9</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1001496</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>10014.959999999999</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1114663</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>11146.63</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1363643</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>13636.43</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1633925</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>16339.25</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1734330</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>17343.3</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2051895</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2213130</v>
+      </c>
+      <c r="E15" s="9">
+        <f>D15/100</f>
+        <v>22131.3</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2446717</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="17">
+        <v>2624477</v>
+      </c>
+      <c r="E16" s="9">
+        <f t="shared" ref="E16:E25" si="1">D16/100</f>
+        <v>26244.77</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9">
+        <v>2978893</v>
+      </c>
+      <c r="E17" s="9">
+        <f t="shared" si="1"/>
+        <v>29788.93</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9">
+        <v>3564238</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" si="1"/>
+        <v>35642.379999999997</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9">
+        <v>3864907</v>
+      </c>
+      <c r="E19" s="9">
+        <f t="shared" si="1"/>
+        <v>38649.07</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9">
+        <v>4364599</v>
+      </c>
+      <c r="E20" s="9">
+        <f t="shared" si="1"/>
+        <v>43645.99</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
+        <v>4890993</v>
+      </c>
+      <c r="E21" s="9">
+        <f t="shared" si="1"/>
+        <v>48909.93</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9">
+        <v>5500545</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" si="1"/>
+        <v>55005.45</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9">
+        <v>6056144</v>
+      </c>
+      <c r="E23" s="9">
+        <f t="shared" si="1"/>
+        <v>60561.440000000002</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9">
+        <v>6617543</v>
+      </c>
+      <c r="E24" s="9">
+        <f t="shared" si="1"/>
+        <v>66175.429999999993</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9">
+        <v>7396074</v>
+      </c>
+      <c r="E25" s="9">
+        <f t="shared" si="1"/>
+        <v>73960.740000000005</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="8">
+        <v>8300254</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="8">
+        <v>95795.12</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9">
+        <v>108884.57</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9">
+        <v>128732.34</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10">
+        <v>151595.9</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10">
+        <v>182522.15</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10">
+        <v>223600.25</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10">
+        <v>260621.28</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="8">
+        <v>298688.33</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="18">
+        <v>297538.52068239864</v>
+      </c>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="8">
+        <v>341351.16</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="18">
+        <v>347032.01266926259</v>
+      </c>
+      <c r="J34" s="19"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="8">
+        <v>388916.63</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="18">
+        <v>399268.11618977698</v>
+      </c>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="18">
+        <v>437144.71134774183</v>
+      </c>
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="18">
+        <v>495504.10640162957</v>
+      </c>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="18">
+        <v>561424.1711553171</v>
+      </c>
+      <c r="J38" s="19"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="18">
+        <v>644963.22063958389</v>
+      </c>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="18">
+        <v>704957.37832466571</v>
+      </c>
+      <c r="J40" s="19"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="18">
+        <v>780612.35380656121</v>
+      </c>
+      <c r="J41" s="19"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="18">
+        <v>764872.40858543455</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>